<commit_message>
dev-1.0.0 : HAV detail dan history
</commit_message>
<xml_diff>
--- a/public/assets/file/Import-HAV.xlsx
+++ b/public/assets/file/Import-HAV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/handika/Documents/02_SOURCE_CODE/01_LARAVEL/04_PHP_8_1/core/public/assets/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF07A58-8C0E-CF49-B655-2B4394B4B02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C4E0D5-F0E9-9949-AE78-0D4C0C599934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{2094B160-FC1C-374C-B708-6E4236F72D07}"/>
   </bookViews>
@@ -1079,99 +1079,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1183,8 +1090,101 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF344C7-1AB6-F042-B540-AF2DFE4B1414}">
   <dimension ref="A1:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -1661,8 +1661,8 @@
     </row>
     <row r="2" spans="1:33">
       <c r="G2" s="2"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
       <c r="AG2" s="52">
         <v>1</v>
       </c>
@@ -1691,26 +1691,26 @@
       </c>
     </row>
     <row r="4" spans="1:33">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
       <c r="AG4" s="52">
         <v>2</v>
       </c>
@@ -1745,19 +1745,19 @@
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
@@ -1772,19 +1772,19 @@
       <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="8"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
@@ -1799,19 +1799,19 @@
       <c r="B8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="8"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="57"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -1826,10 +1826,10 @@
       <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1853,10 +1853,10 @@
       <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1880,19 +1880,19 @@
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="4"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
@@ -1905,17 +1905,17 @@
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="6"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
@@ -1928,17 +1928,17 @@
       <c r="B13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="6"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
     </row>
     <row r="14" spans="1:33" ht="17" thickBot="1">
       <c r="D14" s="12" t="s">
@@ -1974,39 +1974,39 @@
       </c>
     </row>
     <row r="15" spans="1:33" s="14" customFormat="1" ht="17" thickBot="1">
-      <c r="A15" s="72" t="s">
+      <c r="A15" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="74"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="16">
         <f>SUM(D17:D19)/3</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="74"/>
+      <c r="G15" s="63"/>
       <c r="H15" s="16">
         <f>SUM(H17:H23)/7</f>
         <v>0</v>
       </c>
       <c r="I15" s="17"/>
-      <c r="J15" s="72" t="s">
+      <c r="J15" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="73"/>
-      <c r="L15" s="74"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="63"/>
       <c r="M15" s="16">
         <f>SUM(M17:M20)/4</f>
         <v>0</v>
       </c>
       <c r="N15" s="17"/>
-      <c r="O15" s="72" t="s">
+      <c r="O15" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="P15" s="74"/>
+      <c r="P15" s="63"/>
       <c r="Q15" s="16">
         <f>SUM(Q17:Q20)/4</f>
         <v>0</v>
@@ -2058,92 +2058,86 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="104.25" customHeight="1">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="22">
-        <v>5</v>
-      </c>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="80" t="s">
+      <c r="F17" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="81"/>
+      <c r="G17" s="72"/>
       <c r="H17" s="22"/>
       <c r="I17" s="24"/>
-      <c r="J17" s="59" t="s">
+      <c r="J17" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="60"/>
-      <c r="L17" s="61"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="73"/>
       <c r="M17" s="22"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="80" t="s">
+      <c r="O17" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="P17" s="81"/>
+      <c r="P17" s="72"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="24"/>
     </row>
     <row r="18" spans="1:18" ht="110.25" customHeight="1">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="22">
-        <v>5</v>
-      </c>
+      <c r="B18" s="70"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="25"/>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="54"/>
+      <c r="G18" s="75"/>
       <c r="H18" s="22"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="59" t="s">
+      <c r="J18" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="60"/>
-      <c r="L18" s="61"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="73"/>
       <c r="M18" s="22"/>
       <c r="N18" s="24"/>
-      <c r="O18" s="80" t="s">
+      <c r="O18" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="P18" s="81"/>
+      <c r="P18" s="72"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="24"/>
     </row>
     <row r="19" spans="1:18" ht="17" thickBot="1">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="22">
-        <v>5</v>
-      </c>
+      <c r="B19" s="70"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="25"/>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="54"/>
+      <c r="G19" s="75"/>
       <c r="H19" s="22"/>
       <c r="I19" s="24"/>
-      <c r="J19" s="59" t="s">
+      <c r="J19" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="61"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="73"/>
       <c r="M19" s="22"/>
       <c r="N19" s="24"/>
-      <c r="O19" s="80" t="s">
+      <c r="O19" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="P19" s="81"/>
+      <c r="P19" s="72"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="24"/>
     </row>
@@ -2153,23 +2147,23 @@
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="54"/>
+      <c r="G20" s="75"/>
       <c r="H20" s="22"/>
       <c r="I20" s="24"/>
-      <c r="J20" s="69" t="s">
+      <c r="J20" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="70"/>
-      <c r="L20" s="75"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="78"/>
       <c r="M20" s="22"/>
       <c r="N20" s="27"/>
-      <c r="O20" s="76" t="s">
+      <c r="O20" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="P20" s="77"/>
+      <c r="P20" s="80"/>
       <c r="Q20" s="22"/>
       <c r="R20" s="27"/>
     </row>
@@ -2179,14 +2173,14 @@
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="78"/>
+      <c r="G21" s="81"/>
       <c r="H21" s="22"/>
       <c r="I21" s="24"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
       <c r="L21" s="30"/>
       <c r="M21" s="26"/>
       <c r="N21" s="29"/>
@@ -2201,14 +2195,14 @@
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
-      <c r="F22" s="53" t="s">
+      <c r="F22" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="54"/>
+      <c r="G22" s="75"/>
       <c r="H22" s="22"/>
       <c r="I22" s="24"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="79"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
       <c r="L22" s="30"/>
       <c r="M22" s="29"/>
       <c r="N22" s="29"/>
@@ -2223,14 +2217,14 @@
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
-      <c r="F23" s="69" t="s">
+      <c r="F23" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="70"/>
+      <c r="G23" s="77"/>
       <c r="H23" s="22"/>
       <c r="I23" s="27"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="83"/>
       <c r="L23" s="34"/>
       <c r="M23" s="33"/>
       <c r="N23" s="33"/>
@@ -2273,39 +2267,39 @@
       </c>
     </row>
     <row r="25" spans="1:18" s="14" customFormat="1" ht="17" thickBot="1">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="74"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="16">
         <f>SUM(D27:D31)/5</f>
         <v>0</v>
       </c>
       <c r="E25" s="17"/>
-      <c r="F25" s="72" t="s">
+      <c r="F25" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="74"/>
+      <c r="G25" s="63"/>
       <c r="H25" s="16">
         <f>SUM(H27:H36)/10</f>
         <v>0</v>
       </c>
       <c r="I25" s="17"/>
-      <c r="J25" s="72" t="s">
+      <c r="J25" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="73"/>
-      <c r="L25" s="74"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="63"/>
       <c r="M25" s="16">
         <f>SUM(M27:M33)/7</f>
         <v>0</v>
       </c>
       <c r="N25" s="17"/>
-      <c r="O25" s="72" t="s">
+      <c r="O25" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="P25" s="74"/>
+      <c r="P25" s="63"/>
       <c r="Q25" s="16">
         <f>SUM(Q27:Q33)/7</f>
         <v>0</v>
@@ -2357,142 +2351,142 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="55.5" customHeight="1">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="60"/>
-      <c r="C27" s="61"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="73"/>
       <c r="D27" s="22"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="53" t="s">
+      <c r="F27" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="54"/>
+      <c r="G27" s="75"/>
       <c r="H27" s="22"/>
       <c r="I27" s="24"/>
-      <c r="J27" s="59" t="s">
+      <c r="J27" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="60"/>
-      <c r="L27" s="61"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="73"/>
       <c r="M27" s="22"/>
       <c r="N27" s="24"/>
-      <c r="O27" s="53" t="s">
+      <c r="O27" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="P27" s="54"/>
+      <c r="P27" s="75"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="24"/>
     </row>
     <row r="28" spans="1:18" ht="58.5" customHeight="1">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="73"/>
       <c r="D28" s="22"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="53" t="s">
+      <c r="F28" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="54"/>
+      <c r="G28" s="75"/>
       <c r="H28" s="22"/>
       <c r="I28" s="24"/>
-      <c r="J28" s="59" t="s">
+      <c r="J28" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="60"/>
-      <c r="L28" s="61"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="73"/>
       <c r="M28" s="22"/>
       <c r="N28" s="24"/>
-      <c r="O28" s="53" t="s">
+      <c r="O28" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="P28" s="54"/>
+      <c r="P28" s="75"/>
       <c r="Q28" s="22"/>
       <c r="R28" s="24"/>
     </row>
     <row r="29" spans="1:18" ht="63.75" customHeight="1">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="73"/>
       <c r="D29" s="22"/>
       <c r="E29" s="24"/>
-      <c r="F29" s="53" t="s">
+      <c r="F29" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="54"/>
+      <c r="G29" s="75"/>
       <c r="H29" s="22"/>
       <c r="I29" s="24"/>
-      <c r="J29" s="59" t="s">
+      <c r="J29" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="K29" s="60"/>
-      <c r="L29" s="61"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="73"/>
       <c r="M29" s="22"/>
       <c r="N29" s="24"/>
-      <c r="O29" s="53" t="s">
+      <c r="O29" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="P29" s="54"/>
+      <c r="P29" s="75"/>
       <c r="Q29" s="22"/>
       <c r="R29" s="24"/>
     </row>
     <row r="30" spans="1:18" ht="99" customHeight="1">
-      <c r="A30" s="59" t="s">
+      <c r="A30" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="73"/>
       <c r="D30" s="22"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="53" t="s">
+      <c r="F30" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="75"/>
       <c r="H30" s="22"/>
       <c r="I30" s="24"/>
-      <c r="J30" s="59" t="s">
+      <c r="J30" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="K30" s="60"/>
-      <c r="L30" s="61"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="73"/>
       <c r="M30" s="22"/>
       <c r="N30" s="24"/>
-      <c r="O30" s="53" t="s">
+      <c r="O30" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="P30" s="54"/>
+      <c r="P30" s="75"/>
       <c r="Q30" s="22"/>
       <c r="R30" s="24"/>
     </row>
     <row r="31" spans="1:18" ht="17" thickBot="1">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="61"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="22"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="53" t="s">
+      <c r="F31" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="54"/>
+      <c r="G31" s="75"/>
       <c r="H31" s="22"/>
       <c r="I31" s="24"/>
-      <c r="J31" s="59" t="s">
+      <c r="J31" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="K31" s="60"/>
-      <c r="L31" s="61"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="73"/>
       <c r="M31" s="22"/>
       <c r="N31" s="24"/>
-      <c r="O31" s="53" t="s">
+      <c r="O31" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="P31" s="54"/>
+      <c r="P31" s="75"/>
       <c r="Q31" s="22"/>
       <c r="R31" s="24"/>
     </row>
@@ -2502,23 +2496,23 @@
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="29"/>
-      <c r="F32" s="53" t="s">
+      <c r="F32" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="54"/>
+      <c r="G32" s="75"/>
       <c r="H32" s="22"/>
       <c r="I32" s="24"/>
-      <c r="J32" s="59" t="s">
+      <c r="J32" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="K32" s="60"/>
-      <c r="L32" s="61"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="73"/>
       <c r="M32" s="22"/>
       <c r="N32" s="24"/>
-      <c r="O32" s="53" t="s">
+      <c r="O32" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="P32" s="54"/>
+      <c r="P32" s="75"/>
       <c r="Q32" s="22"/>
       <c r="R32" s="24"/>
     </row>
@@ -2528,23 +2522,23 @@
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
-      <c r="F33" s="53" t="s">
+      <c r="F33" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="54"/>
+      <c r="G33" s="75"/>
       <c r="H33" s="22"/>
       <c r="I33" s="24"/>
-      <c r="J33" s="59" t="s">
+      <c r="J33" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="K33" s="60"/>
-      <c r="L33" s="61"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="73"/>
       <c r="M33" s="22"/>
       <c r="N33" s="36"/>
-      <c r="O33" s="62" t="s">
+      <c r="O33" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="P33" s="63"/>
+      <c r="P33" s="87"/>
       <c r="Q33" s="22"/>
       <c r="R33" s="36"/>
     </row>
@@ -2554,10 +2548,10 @@
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
-      <c r="F34" s="53" t="s">
+      <c r="F34" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="54"/>
+      <c r="G34" s="75"/>
       <c r="H34" s="22"/>
       <c r="I34" s="25"/>
       <c r="J34" s="37"/>
@@ -2576,10 +2570,10 @@
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
-      <c r="F35" s="53" t="s">
+      <c r="F35" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="54"/>
+      <c r="G35" s="75"/>
       <c r="H35" s="22"/>
       <c r="I35" s="25"/>
       <c r="J35" s="28"/>
@@ -2598,10 +2592,10 @@
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
-      <c r="F36" s="55" t="s">
+      <c r="F36" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="56"/>
+      <c r="G36" s="85"/>
       <c r="H36" s="22"/>
       <c r="I36" s="39"/>
       <c r="J36" s="32"/>
@@ -2634,8 +2628,8 @@
       <c r="L38" s="42"/>
       <c r="M38" s="43"/>
       <c r="N38" s="44"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
+      <c r="O38" s="59"/>
+      <c r="P38" s="59"/>
     </row>
     <row r="39" spans="1:18">
       <c r="F39" s="45" t="s">
@@ -2673,73 +2667,6 @@
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:R4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="O29:P29"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="F36:G36"/>
@@ -2756,6 +2683,73 @@
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="O30:P30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:R4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="M7:O7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D19 H17:H23 M17:M20 Q17:Q20 D27:D31 H27:H36 M27:M33 Q27:Q33" xr:uid="{6E76B9F4-CAF0-F84F-82EF-E6DAB245AB4E}">

</xml_diff>

<commit_message>
dev-1.0.0 : pindah hav import ke public
</commit_message>
<xml_diff>
--- a/public/assets/file/Import-HAV.xlsx
+++ b/public/assets/file/Import-HAV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/handika/Documents/02_SOURCE_CODE/01_LARAVEL/04_PHP_8_1/core/public/assets/file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/handika/Documents/02_SOURCE_CODE/01_LARAVEL/04_PHP_8_1/core/storage/app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C4E0D5-F0E9-9949-AE78-0D4C0C599934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3322FF-297C-5440-AC01-7A0913380A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{2094B160-FC1C-374C-B708-6E4236F72D07}"/>
   </bookViews>
@@ -35,6 +35,114 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3CF811E8-9591-0C43-9160-B331793A7E31}</author>
+    <author>tc={28CA6143-188C-1F49-B9FC-00FFF8669AC0}</author>
+    <author>tc={9BB9F849-EEDD-9A49-9492-5BCC4926B9B3}</author>
+    <author>tc={4CD1518E-CC30-4E40-9051-DCCEDF5B1B8B}</author>
+    <author>tc={7CB8F079-BE70-EB49-8598-224D6AF4DF1E}</author>
+    <author>tc={0942CA80-8A69-6A4D-83AE-CB27D0384B41}</author>
+    <author>tc={0E951909-67B4-7E41-A7AF-CDAB1C714B70}</author>
+    <author>tc={F8597F6A-39FA-0048-A706-030820ADCC29}</author>
+    <author>tc={21BCDA45-D655-F541-AEF1-E9D48550755D}</author>
+    <author>tc={BB76829A-4164-4B44-820F-F9A5B8329417}</author>
+    <author>tc={E05BFD07-81C6-4447-A340-212EEB323445}</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{3CF811E8-9591-0C43-9160-B331793A7E31}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Harus diisi NPK 6 digit, contoh (000813)</t>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="1" shapeId="0" xr:uid="{28CA6143-188C-1F49-B9FC-00FFF8669AC0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Harus diisi dengan Komentar, contoh “HAV Imam Mahfud 2025”</t>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="2" shapeId="0" xr:uid="{9BB9F849-EEDD-9A49-9492-5BCC4926B9B3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Harus diisi dengan tahun HAV, contoh “2025”</t>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="3" shapeId="0" xr:uid="{4CD1518E-CC30-4E40-9051-DCCEDF5B1B8B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="4" shapeId="0" xr:uid="{7CB8F079-BE70-EB49-8598-224D6AF4DF1E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+    <comment ref="N17" authorId="5" shapeId="0" xr:uid="{0942CA80-8A69-6A4D-83AE-CB27D0384B41}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+    <comment ref="R17" authorId="6" shapeId="0" xr:uid="{0E951909-67B4-7E41-A7AF-CDAB1C714B70}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="7" shapeId="0" xr:uid="{F8597F6A-39FA-0048-A706-030820ADCC29}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+    <comment ref="I27" authorId="8" shapeId="0" xr:uid="{21BCDA45-D655-F541-AEF1-E9D48550755D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+    <comment ref="N27" authorId="9" shapeId="0" xr:uid="{BB76829A-4164-4B44-820F-F9A5B8329417}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+    <comment ref="R27" authorId="10" shapeId="0" xr:uid="{E05BFD07-81C6-4447-A340-212EEB323445}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Evidence boleh kosong</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
   <si>
@@ -59,9 +167,6 @@
     <t xml:space="preserve">Position </t>
   </si>
   <si>
-    <t xml:space="preserve">Sub Gol  </t>
-  </si>
-  <si>
     <t>User Score</t>
   </si>
   <si>
@@ -264,6 +369,9 @@
   </si>
   <si>
     <t>HAV Year</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -273,7 +381,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0_);\(0.0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -343,6 +451,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -364,7 +478,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -373,19 +487,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -612,21 +713,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -662,21 +748,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -835,19 +906,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -894,6 +952,30 @@
       <right/>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -949,135 +1031,204 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1090,101 +1241,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1306,6 +1388,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="HANDIKA /AIIA" id="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" userId="S::0701-AIIA@ap01.aisingroup.com::98a1c18b-cee6-4b1a-914c-99d89a8f5c74" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1623,12 +1711,50 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C7" dT="2025-05-09T06:32:53.71" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{3CF811E8-9591-0C43-9160-B331793A7E31}">
+    <text>Harus diisi NPK 6 digit, contoh (000813)</text>
+  </threadedComment>
+  <threadedComment ref="C12" dT="2025-05-09T06:33:59.58" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{28CA6143-188C-1F49-B9FC-00FFF8669AC0}">
+    <text>Harus diisi dengan Komentar, contoh “HAV Imam Mahfud 2025”</text>
+  </threadedComment>
+  <threadedComment ref="C13" dT="2025-05-09T06:34:42.92" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{9BB9F849-EEDD-9A49-9492-5BCC4926B9B3}">
+    <text>Harus diisi dengan tahun HAV, contoh “2025”</text>
+  </threadedComment>
+  <threadedComment ref="E17" dT="2025-05-16T07:22:35.91" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{4CD1518E-CC30-4E40-9051-DCCEDF5B1B8B}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+  <threadedComment ref="I17" dT="2025-05-16T07:22:41.33" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{7CB8F079-BE70-EB49-8598-224D6AF4DF1E}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+  <threadedComment ref="N17" dT="2025-05-16T07:22:47.61" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{0942CA80-8A69-6A4D-83AE-CB27D0384B41}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+  <threadedComment ref="R17" dT="2025-05-16T07:22:54.96" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{0E951909-67B4-7E41-A7AF-CDAB1C714B70}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+  <threadedComment ref="E27" dT="2025-05-16T07:23:01.74" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{F8597F6A-39FA-0048-A706-030820ADCC29}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+  <threadedComment ref="I27" dT="2025-05-16T07:23:07.25" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{21BCDA45-D655-F541-AEF1-E9D48550755D}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+  <threadedComment ref="N27" dT="2025-05-16T07:23:13.55" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{BB76829A-4164-4B44-820F-F9A5B8329417}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+  <threadedComment ref="R27" dT="2025-05-16T07:23:19.75" personId="{7AD30935-8FBF-0143-9C6A-E76A8AA30282}" id="{E05BFD07-81C6-4447-A340-212EEB323445}">
+    <text>Evidence boleh kosong</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF344C7-1AB6-F042-B540-AF2DFE4B1414}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF344C7-1AB6-F042-B540-AF2DFE4B1414}">
   <dimension ref="A1:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -1655,15 +1781,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
-      <c r="AG1" s="52">
+      <c r="AG1" s="46">
         <v>0.5</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="G2" s="2"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="AG2" s="52">
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
+      <c r="AG2" s="46">
         <v>1</v>
       </c>
     </row>
@@ -1686,32 +1812,32 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="AG3" s="52">
+      <c r="AG3" s="46">
         <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:33">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="AG4" s="52">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="AG4" s="46">
         <v>2</v>
       </c>
     </row>
@@ -1734,7 +1860,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
-      <c r="AG5" s="52">
+      <c r="AG5" s="46">
         <v>2.5</v>
       </c>
     </row>
@@ -1745,50 +1871,50 @@
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="57"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
-      <c r="AG6" s="52">
+      <c r="AG6" s="46">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:33">
       <c r="A7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="8"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-      <c r="AG7" s="52">
+      <c r="AG7" s="46">
         <v>3.5</v>
       </c>
     </row>
@@ -1799,23 +1925,23 @@
       <c r="B8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="8"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
-      <c r="AG8" s="52">
+      <c r="AG8" s="46">
         <v>4</v>
       </c>
     </row>
@@ -1826,10 +1952,10 @@
       <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1842,7 +1968,7 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
-      <c r="AG9" s="52">
+      <c r="AG9" s="46">
         <v>4.5</v>
       </c>
     </row>
@@ -1853,10 +1979,10 @@
       <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1869,7 +1995,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="AG10" s="52">
+      <c r="AG10" s="46">
         <v>5</v>
       </c>
     </row>
@@ -1880,133 +2006,133 @@
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="4"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
-      <c r="AG11" s="52"/>
+      <c r="AG11" s="46"/>
     </row>
     <row r="12" spans="1:33">
       <c r="A12" s="7" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="6"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
-      <c r="AG12" s="51"/>
+      <c r="AG12" s="45"/>
     </row>
     <row r="13" spans="1:33">
       <c r="A13" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="6"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
+      <c r="M13" s="77"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="77"/>
     </row>
     <row r="14" spans="1:33" ht="17" thickBot="1">
       <c r="D14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="R14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R14" s="13" t="s">
+    </row>
+    <row r="15" spans="1:33" s="14" customFormat="1" ht="17" thickBot="1">
+      <c r="A15" s="60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" s="14" customFormat="1" ht="17" thickBot="1">
-      <c r="A15" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="63"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="16">
         <f>SUM(D17:D19)/3</f>
         <v>0</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="61" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="63"/>
+      <c r="F15" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="62"/>
       <c r="H15" s="16">
         <f>SUM(H17:H23)/7</f>
         <v>0</v>
       </c>
       <c r="I15" s="17"/>
-      <c r="J15" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="62"/>
-      <c r="L15" s="63"/>
+      <c r="J15" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="61"/>
+      <c r="L15" s="62"/>
       <c r="M15" s="16">
         <f>SUM(M17:M20)/4</f>
         <v>0</v>
       </c>
       <c r="N15" s="17"/>
-      <c r="O15" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="P15" s="63"/>
+      <c r="O15" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" s="62"/>
       <c r="Q15" s="16">
         <f>SUM(Q17:Q20)/4</f>
         <v>0</v>
@@ -2014,292 +2140,292 @@
       <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:33" s="14" customFormat="1">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="18" t="s">
+      <c r="E16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="59"/>
+      <c r="H16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="64"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="104.25" customHeight="1">
+      <c r="A17" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="68"/>
-      <c r="H16" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="65"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="O16" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="P16" s="68"/>
-      <c r="Q16" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="R16" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="104.25" customHeight="1">
-      <c r="A17" s="69" t="s">
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="71" t="s">
+      <c r="G17" s="75"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="72"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="69" t="s">
+      <c r="K17" s="54"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="70"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="71" t="s">
+      <c r="P17" s="75"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="85"/>
+    </row>
+    <row r="18" spans="1:18" ht="110.25" customHeight="1">
+      <c r="A18" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="24"/>
-    </row>
-    <row r="18" spans="1:18" ht="110.25" customHeight="1">
-      <c r="A18" s="69" t="s">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="74" t="s">
+      <c r="G18" s="48"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="75"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="69" t="s">
+      <c r="K18" s="54"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="70"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="71" t="s">
+      <c r="P18" s="75"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="86"/>
+    </row>
+    <row r="19" spans="1:18" ht="17" thickBot="1">
+      <c r="A19" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="P18" s="72"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="24"/>
-    </row>
-    <row r="19" spans="1:18" ht="17" thickBot="1">
-      <c r="A19" s="69" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="74" t="s">
+      <c r="G19" s="48"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="75"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="69" t="s">
+      <c r="K19" s="54"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="70"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="71" t="s">
+      <c r="P19" s="75"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="86"/>
+    </row>
+    <row r="20" spans="1:18" ht="17" thickBot="1">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="24"/>
-    </row>
-    <row r="20" spans="1:18" ht="17" thickBot="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="74" t="s">
+      <c r="G20" s="48"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="75"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="76" t="s">
+      <c r="K20" s="67"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="77"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="79" t="s">
+      <c r="P20" s="70"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="87"/>
+    </row>
+    <row r="21" spans="1:18" ht="39.75" customHeight="1">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="P20" s="80"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="27"/>
-    </row>
-    <row r="21" spans="1:18" ht="39.75" customHeight="1">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="74" t="s">
+      <c r="G21" s="71"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="27"/>
+    </row>
+    <row r="22" spans="1:18" ht="83.25" customHeight="1">
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="81"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="31"/>
-    </row>
-    <row r="22" spans="1:18" ht="83.25" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="74" t="s">
+      <c r="G22" s="48"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="27"/>
+    </row>
+    <row r="23" spans="1:18" ht="17" thickBot="1">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="75"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="31"/>
-    </row>
-    <row r="23" spans="1:18" ht="17" thickBot="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="76" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="77"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="35"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="31"/>
     </row>
     <row r="24" spans="1:18" ht="17" thickBot="1">
       <c r="D24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="M24" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="N24" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="R24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R24" s="13" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="25" spans="1:18" s="14" customFormat="1" ht="17" thickBot="1">
-      <c r="A25" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="62"/>
-      <c r="C25" s="63"/>
+      <c r="A25" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="16">
         <f>SUM(D27:D31)/5</f>
         <v>0</v>
       </c>
       <c r="E25" s="17"/>
-      <c r="F25" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="63"/>
+      <c r="F25" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="62"/>
       <c r="H25" s="16">
         <f>SUM(H27:H36)/10</f>
         <v>0</v>
       </c>
       <c r="I25" s="17"/>
-      <c r="J25" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="62"/>
-      <c r="L25" s="63"/>
+      <c r="J25" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="61"/>
+      <c r="L25" s="62"/>
       <c r="M25" s="16">
         <f>SUM(M27:M33)/7</f>
         <v>0</v>
       </c>
       <c r="N25" s="17"/>
-      <c r="O25" s="61" t="s">
-        <v>38</v>
-      </c>
-      <c r="P25" s="63"/>
+      <c r="O25" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="P25" s="62"/>
       <c r="Q25" s="16">
         <f>SUM(Q27:Q33)/7</f>
         <v>0</v>
@@ -2307,306 +2433,306 @@
       <c r="R25" s="17"/>
     </row>
     <row r="26" spans="1:18" s="14" customFormat="1">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="64"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="20" t="s">
+      <c r="E26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="67" t="s">
+      <c r="F26" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="59"/>
+      <c r="H26" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="68"/>
-      <c r="H26" s="20" t="s">
+      <c r="I26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="64" t="s">
+      <c r="J26" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="64"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="65"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="20" t="s">
+      <c r="N26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" s="67" t="s">
+      <c r="O26" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="20" t="s">
+      <c r="R26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="R26" s="21" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="27" spans="1:18" ht="55.5" customHeight="1">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="54"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="74" t="s">
+      <c r="G27" s="48"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="75"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="69" t="s">
+      <c r="K27" s="54"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="85"/>
+      <c r="O27" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="70"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="74" t="s">
+      <c r="P27" s="48"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="85"/>
+    </row>
+    <row r="28" spans="1:18" ht="58.5" customHeight="1">
+      <c r="A28" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="P27" s="75"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="24"/>
-    </row>
-    <row r="28" spans="1:18" ht="58.5" customHeight="1">
-      <c r="A28" s="69" t="s">
+      <c r="B28" s="54"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="74" t="s">
+      <c r="G28" s="48"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="75"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="69" t="s">
+      <c r="K28" s="54"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="70"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="74" t="s">
+      <c r="P28" s="48"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="86"/>
+    </row>
+    <row r="29" spans="1:18" ht="63.75" customHeight="1">
+      <c r="A29" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="P28" s="75"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="24"/>
-    </row>
-    <row r="29" spans="1:18" ht="63.75" customHeight="1">
-      <c r="A29" s="69" t="s">
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="74" t="s">
+      <c r="G29" s="48"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="75"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="69" t="s">
+      <c r="K29" s="54"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="K29" s="70"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="74" t="s">
+      <c r="P29" s="48"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="86"/>
+    </row>
+    <row r="30" spans="1:18" ht="99" customHeight="1">
+      <c r="A30" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="24"/>
-    </row>
-    <row r="30" spans="1:18" ht="99" customHeight="1">
-      <c r="A30" s="69" t="s">
+      <c r="B30" s="54"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="74" t="s">
+      <c r="G30" s="48"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="75"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="69" t="s">
+      <c r="K30" s="54"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="K30" s="70"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="74" t="s">
+      <c r="P30" s="48"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="86"/>
+    </row>
+    <row r="31" spans="1:18" ht="17" thickBot="1">
+      <c r="A31" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="P30" s="75"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="24"/>
-    </row>
-    <row r="31" spans="1:18" ht="17" thickBot="1">
-      <c r="A31" s="69" t="s">
+      <c r="B31" s="54"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="74" t="s">
+      <c r="G31" s="48"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="75"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="69" t="s">
+      <c r="K31" s="54"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="K31" s="70"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="74" t="s">
+      <c r="P31" s="48"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="86"/>
+    </row>
+    <row r="32" spans="1:18" ht="54" customHeight="1">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="P31" s="75"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="24"/>
-    </row>
-    <row r="32" spans="1:18" ht="54" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="74" t="s">
+      <c r="G32" s="48"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="75"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="69" t="s">
+      <c r="K32" s="54"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="K32" s="70"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="74" t="s">
+      <c r="P32" s="48"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="86"/>
+    </row>
+    <row r="33" spans="1:18" ht="17" thickBot="1">
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="24"/>
-    </row>
-    <row r="33" spans="1:18" ht="17" thickBot="1">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="74" t="s">
+      <c r="G33" s="48"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="75"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="69" t="s">
+      <c r="K33" s="54"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="87"/>
+      <c r="O33" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="K33" s="70"/>
-      <c r="L33" s="73"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="86" t="s">
+      <c r="P33" s="57"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="87"/>
+    </row>
+    <row r="34" spans="1:18" ht="69.75" customHeight="1">
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="P33" s="87"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="36"/>
-    </row>
-    <row r="34" spans="1:18" ht="69.75" customHeight="1">
-      <c r="A34" s="28"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="74" t="s">
+      <c r="G34" s="48"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="33"/>
+    </row>
+    <row r="35" spans="1:18" ht="69.75" customHeight="1">
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="38"/>
-    </row>
-    <row r="35" spans="1:18" ht="69.75" customHeight="1">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="74" t="s">
+      <c r="G35" s="48"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="86"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="27"/>
+    </row>
+    <row r="36" spans="1:18" ht="17" thickBot="1">
+      <c r="A36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="75"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="31"/>
-    </row>
-    <row r="36" spans="1:18" ht="17" thickBot="1">
-      <c r="A36" s="32"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" s="85"/>
+      <c r="G36" s="50"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33"/>
-      <c r="R36" s="35"/>
+      <c r="I36" s="87"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="31"/>
     </row>
     <row r="37" spans="1:18">
       <c r="F37" s="3"/>
@@ -2615,58 +2741,133 @@
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="F38" s="40" t="s">
+      <c r="F38" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="35"/>
+      <c r="H38" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="F39" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="41"/>
-      <c r="H38" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="44"/>
-      <c r="O38" s="59"/>
-      <c r="P38" s="59"/>
-    </row>
-    <row r="39" spans="1:18">
-      <c r="F39" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="46"/>
+      <c r="G39" s="40"/>
       <c r="H39" s="6" t="s">
         <v>2</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-      <c r="N39" s="47"/>
+      <c r="N39" s="41"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="F40" s="48"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="49"/>
-      <c r="I40" s="49" t="s">
+      <c r="F40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="50"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="83">
+  <mergeCells count="91">
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="I27:I36"/>
+    <mergeCell ref="N27:N33"/>
+    <mergeCell ref="R27:R33"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:R4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="I17:I23"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="O29:P29"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="F36:G36"/>
@@ -2683,73 +2884,6 @@
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="O30:P30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:R4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="M7:O7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D19 H17:H23 M17:M20 Q17:Q20 D27:D31 H27:H36 M27:M33 Q27:Q33" xr:uid="{6E76B9F4-CAF0-F84F-82EF-E6DAB245AB4E}">
@@ -2758,5 +2892,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>